<commit_message>
updated TOBE_Technical_Model.bpmn and added python code
</commit_message>
<xml_diff>
--- a/Python/form_data.xlsx
+++ b/Python/form_data.xlsx
@@ -16,14 +16,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +51,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,29 +429,189 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>submissionid</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>feedbackType</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>query</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>firstName</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>lastName</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>feedbackText</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>needsClarification</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>urgency</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>impactScope</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>forwardToDepartment</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>linkToAdditForm</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>reminderSent</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45778.68244238426</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>be75975c-2697-11f0-a674-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>lorism@gmx.net</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>(078) 715-3999</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Julie</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Eckmann</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Dini mueter</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45778.73738229166</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cb9b5f8d-26a2-11f0-a674-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>loris.marino@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>(078) 715-3999</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Dover</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45778.7507708024</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7c24a12b-26a5-11f0-a674-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>loris.marino@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>(078) 715-3999</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Loris</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Mariño</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>(078) 715-3999</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>lorism@gmx.net</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Das ist die Frage</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added Script for "Supplement Feedback" Task and updated prepare_feedback_supplementation_form.py and send_query_email.py
</commit_message>
<xml_diff>
--- a/Python/form_data.xlsx
+++ b/Python/form_data.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,7 +582,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45778.7507708024</v>
+        <v>45778.75077079861</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -612,6 +612,416 @@
       <c r="I4" t="inlineStr">
         <is>
           <t>Das ist die Frage</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45789.37653412037</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>e7a95397-2efe-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>john@example.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45789.3798040162</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>aeb3eab1-2eff-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>john@example.com</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45789.3834979051</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>6a36d908-2f00-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>john@example.com</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>+41312</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45789.4085253125</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>74fdb053-2f05-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45789.41376583333</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8348a2fa-2f06-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>john@example.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>+41312</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45789.41448775463</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>a8f0fcc1-2f06-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45789.41756166667</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>44d6f554-2f07-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>john@example.com</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>+41312</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45789.41876859953</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>835e7f6f-2f07-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45789.45248675926</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>4d646cfe-2f0e-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45789.47321222222</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>76ca6e57-2f12-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45789.51575185185</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>06adef80-2f1b-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Smith</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45789.51829799668</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>8ae1c6ae-2f1b-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>kevin.maier@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>312312</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Olaf</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Schulz</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Aenean mollis ultricies interdum. Nullam pharetra vitae lectus eget volutpat. Integer in sodales ligula. Vestibulum pellentesque arcu in est aliquam rhoncus. Curabitur et dui quis arcu scelerisque congue. Pellentesque libero ligula, sagittis a tempus quis, finibus eget erat. Nunc sed tempor nunc. Mauris tempor odio id lorem commodo dapibus. Nulla viverra mi in magna imperdiet volutpat.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
try previous push again
</commit_message>
<xml_diff>
--- a/Python/form_data.xlsx
+++ b/Python/form_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,6 +618,80 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>f34630c2-31aa-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>15.05.2025</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>loris.marino@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>41787153999</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Hans</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Volter</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Many have tried to interfere with my work. You think you are somehow better?</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>140a4b37-31ac-11f0-8dd5-fa163ee583d0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>15.05.2025</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>loris.marino@students.fhnw.ch</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>41787153999</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Loris</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Mariño</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Feedback Feedback DASSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSSasda sdjasdi asdjasd asd adihsdifhse IFESUFH SEIUFHESUFH SEIFSEIFH SEIIUFHUD SDLJHSDK JVHKJ YDkjefsdkjfh sifhsduf hsfhefsdv90shgw89ej f9sdv9'ah erduvi sdfgnraivndf ipdufn ipjdfn era9u a9erngijsdvnpiagh 9'a4eugaidrug iardug 'a8eugiuergn rghaergnuaer giuaeug aegaerug hae9rghae9r greg oyidjk&lt;setm nbglkdifjvpiuvpiruagh98a hyidnvpivjpiaegh a iaug aerg raiugidugh a'ivfdipghea</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>